<commit_message>
1.  Set up relay_parameters.xlsx to accommodate load 2 without tripping
</commit_message>
<xml_diff>
--- a/Components/SimulinkOpal/CHPandThermal/relay_settings/relay_parameters.xlsx
+++ b/Components/SimulinkOpal/CHPandThermal/relay_settings/relay_parameters.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +917,7 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="7">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>

</xml_diff>